<commit_message>
Test values for battery storage potential
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamho\Dropbox\Energy Innovation\InputData_RevisionRequest\elec\GBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CB9762-BBC9-437D-BE59-63676D1B60C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2AF3CF-C87A-48B8-99FC-634CA6998C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13350" yWindow="440" windowWidth="22630" windowHeight="20520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="18-20_Cap" sheetId="16" r:id="rId2"/>
     <sheet name="20-50_Cap" sheetId="18" r:id="rId3"/>
-    <sheet name="AEO Table 9 (2019)" sheetId="8" state="hidden" r:id="rId4"/>
-    <sheet name="BGBSC" sheetId="3" r:id="rId5"/>
-    <sheet name="PAGBSC" sheetId="5" r:id="rId6"/>
-    <sheet name="SYGBSC" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="19" r:id="rId4"/>
+    <sheet name="AEO Table 9 (2019)" sheetId="8" state="hidden" r:id="rId5"/>
+    <sheet name="BGBSC" sheetId="3" r:id="rId6"/>
+    <sheet name="PAGBSC" sheetId="5" r:id="rId7"/>
+    <sheet name="SYGBSC" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="gigwatts_to_megawatts">About!$A$37</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="185">
   <si>
     <t>Source:</t>
   </si>
@@ -650,6 +651,9 @@
   <si>
     <t>Peak reduction plan - ESS (2020~2034)</t>
     <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>Additional Potential (GW)</t>
   </si>
 </sst>
 </file>
@@ -657,15 +661,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="177" formatCode="#,##0.0"/>
-    <numFmt numFmtId="178" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -673,7 +677,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -681,7 +685,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -841,13 +845,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -855,7 +859,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -863,7 +867,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -872,7 +876,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -881,7 +885,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1184,7 +1188,7 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1269,26 +1273,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="56" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="11" xfId="55" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="11" xfId="55" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="11" xfId="55" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="11" xfId="55" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="56" applyFont="1" applyFill="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="17" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="17" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="17" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="17" borderId="12" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
@@ -1380,9 +1384,11 @@
     <cellStyle name="Heading 2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="Heading 3 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Heading 4 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Input 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
     <cellStyle name="Linked Cell 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Neutral 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="Normal 2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
     <cellStyle name="Normal 2 3" xfId="48" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
@@ -1401,8 +1407,6 @@
     <cellStyle name="Title 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
     <cellStyle name="Total 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
     <cellStyle name="Warning Text 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1418,7 +1422,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1740,32 +1744,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="60.75" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="60.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" s="6" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" s="6" customFormat="1">
       <c r="A3" s="7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1773,120 +1777,120 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="B6" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2">
       <c r="B7" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2">
       <c r="B8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2">
       <c r="B9" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2">
       <c r="B10" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2">
       <c r="B12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2">
       <c r="B13" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" s="6" customFormat="1">
       <c r="B14" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2">
       <c r="B15" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" s="6" customFormat="1"/>
+    <row r="17" spans="1:2" s="6" customFormat="1">
       <c r="B17" s="6" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" s="6" customFormat="1">
       <c r="B18" s="3">
         <v>2020</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" s="6" customFormat="1">
       <c r="B19" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" s="6" customFormat="1">
       <c r="B20" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="22" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" s="6" customFormat="1"/>
+    <row r="22" spans="1:2" s="6" customFormat="1">
       <c r="B22" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" s="6" customFormat="1">
       <c r="B23" s="6" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" s="6" customFormat="1">
       <c r="B24" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" s="6" customFormat="1">
       <c r="B25" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2">
       <c r="B26" s="45" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" s="6" customFormat="1"/>
+    <row r="31" spans="1:2">
       <c r="A31" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2">
       <c r="A34" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B34" s="6"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2">
       <c r="A37" s="3"/>
       <c r="B37" s="6"/>
     </row>
@@ -1909,21 +1913,21 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="11.58203125" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="5" max="5" width="12.58203125" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
     <col min="6" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9">
       <c r="C4" t="s">
         <v>156</v>
       </c>
@@ -1940,7 +1944,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="34" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" ht="29">
       <c r="B5" s="28" t="s">
         <v>162</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="34" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" ht="29">
       <c r="B6" s="28" t="s">
         <v>161</v>
       </c>
@@ -1980,7 +1984,7 @@
         <v>4773</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9">
       <c r="B8" s="33" t="s">
         <v>164</v>
       </c>
@@ -2005,7 +2009,7 @@
         <v>2.9738317757009347</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9">
       <c r="C13">
         <v>2019</v>
       </c>
@@ -2022,7 +2026,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9">
       <c r="B14" t="s">
         <v>166</v>
       </c>
@@ -2044,12 +2048,12 @@
         <v>2560.3333333333335</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9">
       <c r="B16" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
         <v>167</v>
       </c>
@@ -2058,7 +2062,7 @@
         <v>4.8658743633276744</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
         <v>168</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:3">
       <c r="B20" s="36" t="s">
         <v>169</v>
       </c>
@@ -2084,21 +2088,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA08D23-6BBE-4AD0-B993-956F6C797274}">
   <dimension ref="B2:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:33" ht="25.5" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:33" ht="21">
       <c r="B2" s="42" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="2:33" ht="21" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:33" ht="18.5">
       <c r="R3" s="40"/>
       <c r="S3" s="41"/>
       <c r="T3" s="41"/>
@@ -2116,7 +2120,7 @@
       <c r="AF3" s="41"/>
       <c r="AG3" s="41"/>
     </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:33">
       <c r="C4">
         <v>2020</v>
       </c>
@@ -2211,7 +2215,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:33">
       <c r="C5">
         <v>105</v>
       </c>
@@ -2322,7 +2326,7 @@
         <v>2831.4131751078003</v>
       </c>
     </row>
-    <row r="7" spans="2:33" ht="34" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:33" ht="29">
       <c r="B7" s="43" t="s">
         <v>173</v>
       </c>
@@ -2450,7 +2454,7 @@
         <v>3.9417294386824602E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:33">
       <c r="R8" s="38" t="s">
         <v>171</v>
       </c>
@@ -2459,7 +2463,7 @@
       <c r="U8" s="38"/>
       <c r="V8" s="38"/>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:33">
       <c r="B9" t="s">
         <v>175</v>
       </c>
@@ -2581,7 +2585,7 @@
         <v>-0.41364773442397862</v>
       </c>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:33">
       <c r="B11" s="44" t="s">
         <v>145</v>
       </c>
@@ -2679,7 +2683,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:33">
       <c r="B12" s="33" t="s">
         <v>174</v>
       </c>
@@ -2808,7 +2812,7 @@
         <v>27186.441512750134</v>
       </c>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:33">
       <c r="B14" s="6" t="s">
         <v>156</v>
       </c>
@@ -2937,7 +2941,7 @@
         <v>10874.576605100056</v>
       </c>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:33">
       <c r="B15" s="6" t="s">
         <v>157</v>
       </c>
@@ -3066,7 +3070,7 @@
         <v>9671.9365132587718</v>
       </c>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:33">
       <c r="B16" s="6" t="s">
         <v>158</v>
       </c>
@@ -3195,7 +3199,7 @@
         <v>6368.9109089059502</v>
       </c>
     </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:33">
       <c r="B17" s="6" t="s">
         <v>159</v>
       </c>
@@ -3332,6 +3336,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0901BFDC-7419-499F-8451-F914B4698FB9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2050</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK114"/>
   <sheetViews>
@@ -3339,16 +3379,16 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08203125" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.08203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="45.75" style="6" customWidth="1"/>
-    <col min="3" max="37" width="9.08203125" style="6"/>
+    <col min="1" max="1" width="32.08984375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" style="6" customWidth="1"/>
+    <col min="3" max="37" width="9.08984375" style="6"/>
     <col min="38" max="38" width="8" style="6" customWidth="1"/>
-    <col min="39" max="16384" width="9.08203125" style="6"/>
+    <col min="39" max="16384" width="9.08984375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="B1" s="13" t="s">
         <v>127</v>
       </c>
@@ -3455,8 +3495,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1">
       <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
@@ -3467,7 +3507,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:37" ht="15" customHeight="1">
       <c r="C4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3480,7 +3520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:37" ht="15" customHeight="1">
       <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
@@ -3491,7 +3531,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:37" ht="15" customHeight="1">
       <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
@@ -3502,7 +3542,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
@@ -3510,12 +3550,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:37" ht="15" customHeight="1">
       <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:37" ht="15" customHeight="1">
       <c r="B12" s="13" t="s">
         <v>10</v>
       </c>
@@ -3625,7 +3665,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="B13" s="14" t="s">
         <v>11</v>
       </c>
@@ -3735,18 +3775,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1"/>
+    <row r="15" spans="1:37" ht="15" customHeight="1">
       <c r="B15" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:37" ht="15" customHeight="1">
       <c r="B16" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:37" ht="15" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
@@ -3859,7 +3899,7 @@
         <v>-1.4527999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:37" ht="15" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
@@ -3972,7 +4012,7 @@
         <v>-1.2109E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:37" ht="15" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
@@ -4085,7 +4125,7 @@
         <v>2.2502999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:37" ht="15" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>20</v>
       </c>
@@ -4198,7 +4238,7 @@
         <v>8.456E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:37" ht="15" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>22</v>
       </c>
@@ -4311,7 +4351,7 @@
         <v>-5.6340000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:37" ht="15" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>24</v>
       </c>
@@ -4424,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:37" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="22" t="s">
         <v>26</v>
       </c>
@@ -4537,7 +4577,7 @@
         <v>0.123014</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" ht="15" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>28</v>
       </c>
@@ -4650,7 +4690,7 @@
         <v>5.8900000000000003E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:37" ht="15" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>30</v>
       </c>
@@ -4763,7 +4803,7 @@
         <v>2.3185000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:37" ht="15" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>32</v>
       </c>
@@ -4876,7 +4916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>35</v>
       </c>
@@ -4989,12 +5029,12 @@
         <v>1.1344E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:37" ht="15" customHeight="1">
       <c r="B28" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" ht="15" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>38</v>
       </c>
@@ -5107,7 +5147,7 @@
         <v>-3.3660000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" ht="15" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>40</v>
       </c>
@@ -5220,7 +5260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" ht="15" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>42</v>
       </c>
@@ -5333,7 +5373,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" ht="15" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>43</v>
       </c>
@@ -5446,7 +5486,7 @@
         <v>-9.68E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:37" ht="15" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>44</v>
       </c>
@@ -5559,7 +5599,7 @@
         <v>6.6000000000000005E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:37" ht="15" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>45</v>
       </c>
@@ -5672,12 +5712,12 @@
         <v>-4.06E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:37" ht="15" customHeight="1">
       <c r="B36" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:37" ht="15" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>47</v>
       </c>
@@ -5790,7 +5830,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:37" ht="15" customHeight="1">
       <c r="A38" s="10" t="s">
         <v>48</v>
       </c>
@@ -5903,7 +5943,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:37" ht="15" customHeight="1">
       <c r="A39" s="10" t="s">
         <v>49</v>
       </c>
@@ -6016,7 +6056,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="10" t="s">
         <v>50</v>
       </c>
@@ -6129,7 +6169,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:37" ht="15" customHeight="1">
       <c r="A41" s="10" t="s">
         <v>51</v>
       </c>
@@ -6242,7 +6282,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="10" t="s">
         <v>53</v>
       </c>
@@ -6355,7 +6395,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="10" t="s">
         <v>54</v>
       </c>
@@ -6468,7 +6508,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="10" t="s">
         <v>55</v>
       </c>
@@ -6581,7 +6621,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="10" t="s">
         <v>56</v>
       </c>
@@ -6694,7 +6734,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="10" t="s">
         <v>57</v>
       </c>
@@ -6807,7 +6847,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:37" ht="15" customHeight="1">
       <c r="A47" s="10" t="s">
         <v>59</v>
       </c>
@@ -6920,12 +6960,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:37" ht="15" customHeight="1">
       <c r="B48" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:37" ht="15" customHeight="1">
       <c r="A49" s="10" t="s">
         <v>61</v>
       </c>
@@ -7038,7 +7078,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:37" ht="15" customHeight="1">
       <c r="A50" s="10" t="s">
         <v>62</v>
       </c>
@@ -7151,7 +7191,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:37" ht="15" customHeight="1">
       <c r="A51" s="10" t="s">
         <v>63</v>
       </c>
@@ -7264,7 +7304,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:37" ht="15" customHeight="1">
       <c r="A52" s="10" t="s">
         <v>64</v>
       </c>
@@ -7377,7 +7417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:37" ht="15" customHeight="1">
       <c r="A53" s="10" t="s">
         <v>65</v>
       </c>
@@ -7490,7 +7530,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:37" ht="15" customHeight="1">
       <c r="A54" s="10" t="s">
         <v>66</v>
       </c>
@@ -7603,7 +7643,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:37" ht="15" customHeight="1">
       <c r="A55" s="10" t="s">
         <v>67</v>
       </c>
@@ -7716,7 +7756,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:37" ht="15" customHeight="1">
       <c r="A56" s="10" t="s">
         <v>68</v>
       </c>
@@ -7829,7 +7869,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:37" ht="15" customHeight="1">
       <c r="A57" s="10" t="s">
         <v>69</v>
       </c>
@@ -7942,7 +7982,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:37" ht="15" customHeight="1">
       <c r="A58" s="10" t="s">
         <v>70</v>
       </c>
@@ -8055,7 +8095,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:37" ht="15" customHeight="1">
       <c r="A59" s="10" t="s">
         <v>71</v>
       </c>
@@ -8168,7 +8208,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:37" ht="15" customHeight="1">
       <c r="A60" s="10" t="s">
         <v>72</v>
       </c>
@@ -8281,12 +8321,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:37" ht="15" customHeight="1">
       <c r="B62" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:37" ht="15" customHeight="1">
       <c r="A63" s="10" t="s">
         <v>74</v>
       </c>
@@ -8399,7 +8439,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:37" ht="15" customHeight="1">
       <c r="A64" s="10" t="s">
         <v>75</v>
       </c>
@@ -8512,7 +8552,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:37" ht="15" customHeight="1">
       <c r="A65" s="10" t="s">
         <v>76</v>
       </c>
@@ -8625,7 +8665,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:37" ht="15" customHeight="1">
       <c r="A66" s="10" t="s">
         <v>77</v>
       </c>
@@ -8738,7 +8778,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:37" ht="15" customHeight="1">
       <c r="A67" s="10" t="s">
         <v>78</v>
       </c>
@@ -8851,7 +8891,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:37" ht="15" customHeight="1">
       <c r="A68" s="10" t="s">
         <v>79</v>
       </c>
@@ -8964,7 +9004,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:37" ht="15" customHeight="1">
       <c r="A69" s="10" t="s">
         <v>80</v>
       </c>
@@ -9077,7 +9117,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:37" ht="15" customHeight="1">
       <c r="A70" s="10" t="s">
         <v>81</v>
       </c>
@@ -9190,7 +9230,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:37" ht="15" customHeight="1">
       <c r="A71" s="10" t="s">
         <v>82</v>
       </c>
@@ -9303,7 +9343,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:37" ht="15" customHeight="1">
       <c r="A72" s="10" t="s">
         <v>83</v>
       </c>
@@ -9416,7 +9456,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:37" ht="15" customHeight="1">
       <c r="A74" s="10" t="s">
         <v>84</v>
       </c>
@@ -9529,12 +9569,12 @@
         <v>1.1053E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:37" ht="15" customHeight="1">
       <c r="B76" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:37" ht="15" customHeight="1">
       <c r="A77" s="10" t="s">
         <v>87</v>
       </c>
@@ -9647,7 +9687,7 @@
         <v>-9.3640000000000008E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:37" ht="15" customHeight="1">
       <c r="A78" s="10" t="s">
         <v>88</v>
       </c>
@@ -9760,7 +9800,7 @@
         <v>-2.039E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:37" ht="15" customHeight="1">
       <c r="A79" s="10" t="s">
         <v>90</v>
       </c>
@@ -9873,7 +9913,7 @@
         <v>2.5253000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:37" ht="15" customHeight="1">
       <c r="A80" s="10" t="s">
         <v>92</v>
       </c>
@@ -9986,7 +10026,7 @@
         <v>-7.0799999999999997E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:37" ht="15" customHeight="1">
       <c r="A81" s="10" t="s">
         <v>94</v>
       </c>
@@ -10099,7 +10139,7 @@
         <v>6.0502E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:37" ht="15" customHeight="1">
       <c r="A82" s="10" t="s">
         <v>95</v>
       </c>
@@ -10212,7 +10252,7 @@
         <v>4.0169999999999997E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:37" ht="15" customHeight="1">
       <c r="A83" s="10" t="s">
         <v>97</v>
       </c>
@@ -10325,7 +10365,7 @@
         <v>4.7788999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:37" ht="15" customHeight="1">
       <c r="A85" s="10" t="s">
         <v>98</v>
       </c>
@@ -10438,8 +10478,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="87" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1"/>
+    <row r="87" spans="1:37" ht="15" customHeight="1">
       <c r="B87" s="46" t="s">
         <v>100</v>
       </c>
@@ -10479,137 +10519,137 @@
       <c r="AJ87" s="46"/>
       <c r="AK87" s="46"/>
     </row>
-    <row r="88" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:37" ht="15" customHeight="1">
       <c r="B88" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="89" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:37" ht="15" customHeight="1">
       <c r="B89" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:37" ht="15" customHeight="1">
       <c r="B90" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:37" ht="15" customHeight="1">
       <c r="B91" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:37" ht="15" customHeight="1">
       <c r="B92" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="93" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:37" ht="15" customHeight="1">
       <c r="B93" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:37" ht="15" customHeight="1">
       <c r="B94" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="95" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:37" ht="15" customHeight="1">
       <c r="B95" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="96" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:37" ht="15" customHeight="1">
       <c r="B96" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:2" ht="15" customHeight="1">
       <c r="B97" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:2" ht="15" customHeight="1">
       <c r="B98" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:2" ht="15" customHeight="1">
       <c r="B99" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:2" ht="15" customHeight="1">
       <c r="B100" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:2" ht="15" customHeight="1">
       <c r="B101" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:2" ht="15" customHeight="1">
       <c r="B102" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:2" ht="15" customHeight="1">
       <c r="B103" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:2" ht="15" customHeight="1">
       <c r="B104" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:2" ht="15" customHeight="1">
       <c r="B105" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:2" ht="15" customHeight="1">
       <c r="B106" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:2" ht="15" customHeight="1">
       <c r="B107" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:2" ht="15" customHeight="1">
       <c r="B108" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:2" ht="15" customHeight="1">
       <c r="B109" s="11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:2" ht="15" customHeight="1">
       <c r="B110" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:2" ht="15" customHeight="1">
       <c r="B111" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:2" ht="15" customHeight="1">
       <c r="B112" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:2" ht="15" customHeight="1">
       <c r="B113" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:2" ht="15" customHeight="1">
       <c r="B114" s="11" t="s">
         <v>142</v>
       </c>
@@ -10623,23 +10663,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="33.08203125" customWidth="1"/>
+    <col min="1" max="1" width="33.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32">
       <c r="A1" s="12" t="s">
         <v>122</v>
       </c>
@@ -10737,7 +10777,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -10873,7 +10913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -10881,16 +10921,16 @@
   <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B2" sqref="B2:AF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="47.08203125" customWidth="1"/>
-    <col min="2" max="32" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.08984375" customWidth="1"/>
+    <col min="2" max="32" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32">
       <c r="A1" s="12" t="s">
         <v>122</v>
       </c>
@@ -10988,139 +11028,139 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>123</v>
       </c>
       <c r="B2" s="8" cm="1">
-        <f t="array" ref="B2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!B1)-BGBSC!B2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!B1)-BGBSC!B2),0))</f>
+        <f t="array" ref="B2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!B1)*1000</f>
         <v>0</v>
       </c>
       <c r="C2" s="8" cm="1">
-        <f t="array" ref="C2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!C1)-BGBSC!C2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!C1)-BGBSC!C2),0))</f>
-        <v>0</v>
+        <f t="array" ref="C2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!C1)*1000</f>
+        <v>1666.6666666665151</v>
       </c>
       <c r="D2" s="8" cm="1">
-        <f t="array" ref="D2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!D1)-BGBSC!D2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!D1)-BGBSC!D2),0))</f>
-        <v>0</v>
+        <f t="array" ref="D2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!D1)*1000</f>
+        <v>3333.3333333330302</v>
       </c>
       <c r="E2" s="8" cm="1">
-        <f t="array" ref="E2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!E1)-BGBSC!E2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!E1)-BGBSC!E2),0))</f>
-        <v>0</v>
+        <f t="array" ref="E2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!E1)*1000</f>
+        <v>5000</v>
       </c>
       <c r="F2" s="8" cm="1">
-        <f t="array" ref="F2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!F1)-BGBSC!F2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!F1)-BGBSC!F2),0))</f>
-        <v>210.34153917192134</v>
+        <f t="array" ref="F2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!F1)*1000</f>
+        <v>6666.6666666665151</v>
       </c>
       <c r="G2" s="8" cm="1">
-        <f t="array" ref="G2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!G1)-BGBSC!G2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!G1)-BGBSC!G2),0))</f>
-        <v>1241.0825307006844</v>
+        <f t="array" ref="G2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!G1)*1000</f>
+        <v>8333.3333333330302</v>
       </c>
       <c r="H2" s="8" cm="1">
-        <f t="array" ref="H2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!H1)-BGBSC!H2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!H1)-BGBSC!H2),0))</f>
-        <v>2261.0054514863177</v>
+        <f t="array" ref="H2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!H1)*1000</f>
+        <v>10000</v>
       </c>
       <c r="I2" s="8" cm="1">
-        <f t="array" ref="I2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!I1)-BGBSC!I2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!I1)-BGBSC!I2),0))</f>
-        <v>2285.6658638607105</v>
+        <f t="array" ref="I2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!I1)*1000</f>
+        <v>11666.666666666515</v>
       </c>
       <c r="J2" s="8" cm="1">
-        <f t="array" ref="J2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!J1)-BGBSC!J2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!J1)-BGBSC!J2),0))</f>
-        <v>2072.328719876471</v>
+        <f t="array" ref="J2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!J1)*1000</f>
+        <v>13333.33333333303</v>
       </c>
       <c r="K2" s="8" cm="1">
-        <f t="array" ref="K2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!K1)-BGBSC!K2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!K1)-BGBSC!K2),0))</f>
-        <v>1610.1759487895379</v>
+        <f t="array" ref="K2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!K1)*1000</f>
+        <v>15000</v>
       </c>
       <c r="L2" s="8" cm="1">
-        <f t="array" ref="L2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!L1)-BGBSC!L2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!L1)-BGBSC!L2),0))</f>
-        <v>931.66176283023196</v>
+        <f t="array" ref="L2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!L1)*1000</f>
+        <v>16666.666666666515</v>
       </c>
       <c r="M2" s="8" cm="1">
-        <f t="array" ref="M2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!M1)-BGBSC!M2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!M1)-BGBSC!M2),0))</f>
-        <v>90.876515717460279</v>
+        <f t="array" ref="M2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!M1)*1000</f>
+        <v>18333.33333333303</v>
       </c>
       <c r="N2" s="8" cm="1">
-        <f t="array" ref="N2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!N1)-BGBSC!N2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!N1)-BGBSC!N2),0))</f>
-        <v>0</v>
+        <f t="array" ref="N2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!N1)*1000</f>
+        <v>20000</v>
       </c>
       <c r="O2" s="8" cm="1">
-        <f t="array" ref="O2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!O1)-BGBSC!O2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!O1)-BGBSC!O2),0))</f>
-        <v>0</v>
+        <f t="array" ref="O2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!O1)*1000</f>
+        <v>21666.666666666515</v>
       </c>
       <c r="P2" s="8" cm="1">
-        <f t="array" ref="P2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!P1)-BGBSC!P2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!P1)-BGBSC!P2),0))</f>
-        <v>0</v>
+        <f t="array" ref="P2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!P1)*1000</f>
+        <v>23333.33333333303</v>
       </c>
       <c r="Q2" s="8" cm="1">
-        <f t="array" ref="Q2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!Q1)-BGBSC!Q2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!Q1)-BGBSC!Q2),0))</f>
-        <v>0</v>
+        <f t="array" ref="Q2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!Q1)*1000</f>
+        <v>25000</v>
       </c>
       <c r="R2" s="8" cm="1">
-        <f t="array" ref="R2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!R1)-BGBSC!R2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!R1)-BGBSC!R2),0))</f>
-        <v>0</v>
+        <f t="array" ref="R2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!R1)*1000</f>
+        <v>26666.666666666515</v>
       </c>
       <c r="S2" s="8" cm="1">
-        <f t="array" ref="S2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!S1)-BGBSC!S2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!S1)-BGBSC!S2),0))</f>
-        <v>0</v>
+        <f t="array" ref="S2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!S1)*1000</f>
+        <v>28333.33333333303</v>
       </c>
       <c r="T2" s="8" cm="1">
-        <f t="array" ref="T2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!T1)-BGBSC!T2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!T1)-BGBSC!T2),0))</f>
-        <v>0</v>
+        <f t="array" ref="T2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!T1)*1000</f>
+        <v>30000</v>
       </c>
       <c r="U2" s="8" cm="1">
-        <f t="array" ref="U2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!U1)-BGBSC!U2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!U1)-BGBSC!U2),0))</f>
-        <v>0</v>
+        <f t="array" ref="U2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!U1)*1000</f>
+        <v>31666.666666666515</v>
       </c>
       <c r="V2" s="8" cm="1">
-        <f t="array" ref="V2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!V1)-BGBSC!V2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!V1)-BGBSC!V2),0))</f>
-        <v>0</v>
+        <f t="array" ref="V2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!V1)*1000</f>
+        <v>33333.33333333303</v>
       </c>
       <c r="W2" s="8" cm="1">
-        <f t="array" ref="W2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!W1)-BGBSC!W2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!W1)-BGBSC!W2),0))</f>
-        <v>0</v>
+        <f t="array" ref="W2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!W1)*1000</f>
+        <v>35000</v>
       </c>
       <c r="X2" s="8" cm="1">
-        <f t="array" ref="X2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!X1)-BGBSC!X2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!X1)-BGBSC!X2),0))</f>
-        <v>0</v>
+        <f t="array" ref="X2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!X1)*1000</f>
+        <v>36666.666666666511</v>
       </c>
       <c r="Y2" s="8" cm="1">
-        <f t="array" ref="Y2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!Y1)-BGBSC!Y2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!Y1)-BGBSC!Y2),0))</f>
-        <v>0</v>
+        <f t="array" ref="Y2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!Y1)*1000</f>
+        <v>38333.33333333303</v>
       </c>
       <c r="Z2" s="8" cm="1">
-        <f t="array" ref="Z2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!Z1)-BGBSC!Z2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!Z1)-BGBSC!Z2),0))</f>
-        <v>401.90993807883569</v>
+        <f t="array" ref="Z2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!Z1)*1000</f>
+        <v>40000</v>
       </c>
       <c r="AA2" s="8" cm="1">
-        <f t="array" ref="AA2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AA1)-BGBSC!AA2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AA1)-BGBSC!AA2),0))</f>
-        <v>1475.8624625498087</v>
+        <f t="array" ref="AA2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AA1)*1000</f>
+        <v>41666.666666666511</v>
       </c>
       <c r="AB2" s="8" cm="1">
-        <f t="array" ref="AB2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AB1)-BGBSC!AB2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AB1)-BGBSC!AB2),0))</f>
-        <v>2591.4735343075372</v>
+        <f t="array" ref="AB2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AB1)*1000</f>
+        <v>43333.33333333303</v>
       </c>
       <c r="AC2" s="8" cm="1">
-        <f t="array" ref="AC2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AC1)-BGBSC!AC2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AC1)-BGBSC!AC2),0))</f>
-        <v>3735.4267358947909</v>
+        <f t="array" ref="AC2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AC1)*1000</f>
+        <v>45000</v>
       </c>
       <c r="AD2" s="8" cm="1">
-        <f t="array" ref="AD2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AD1)-BGBSC!AD2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AD1)-BGBSC!AD2),0))</f>
-        <v>4898.1247406487491</v>
+        <f t="array" ref="AD2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AD1)*1000</f>
+        <v>46666.666666666511</v>
       </c>
       <c r="AE2" s="8" cm="1">
-        <f t="array" ref="AE2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AE1)-BGBSC!AE2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AE1)-BGBSC!AE2),0))</f>
-        <v>6072.8802916724635</v>
+        <f t="array" ref="AE2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AE1)*1000</f>
+        <v>48333.33333333303</v>
       </c>
       <c r="AF2" s="8" cm="1">
-        <f t="array" ref="AF2">_xlfn.SINGLE(IF((TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AF1)-BGBSC!AF2)&gt;0,(TREND('20-50_Cap'!$D$12:$Q$12,'20-50_Cap'!$D$11:$Q$11,PAGBSC!AF1)-BGBSC!AF2),0))</f>
-        <v>7255.1804070266444</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+        <f t="array" ref="AF2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AF1)*1000</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32">
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32">
       <c r="D6" s="6"/>
     </row>
   </sheetData>
@@ -11130,7 +11170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -11141,14 +11181,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08203125" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9.08203125" style="6"/>
+    <col min="1" max="1" width="11.36328125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="9.08984375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
         <v>122</v>
       </c>
@@ -11156,7 +11196,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>126</v>
       </c>
@@ -11165,7 +11205,7 @@
         <v>2381.9179400113185</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="B3" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set potential battery storage equal to double BAU
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2AF3CF-C87A-48B8-99FC-634CA6998C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C12715-B2D6-48D9-BF3D-9A4807E530ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="18-20_Cap" sheetId="16" r:id="rId2"/>
     <sheet name="20-50_Cap" sheetId="18" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="19" r:id="rId4"/>
-    <sheet name="AEO Table 9 (2019)" sheetId="8" state="hidden" r:id="rId5"/>
-    <sheet name="BGBSC" sheetId="3" r:id="rId6"/>
-    <sheet name="PAGBSC" sheetId="5" r:id="rId7"/>
-    <sheet name="SYGBSC" sheetId="9" r:id="rId8"/>
+    <sheet name="AEO Table 9 (2019)" sheetId="8" state="hidden" r:id="rId4"/>
+    <sheet name="BGBSC" sheetId="3" r:id="rId5"/>
+    <sheet name="PAGBSC" sheetId="5" r:id="rId6"/>
+    <sheet name="SYGBSC" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="gigwatts_to_megawatts">About!$A$37</definedName>
@@ -40,28 +39,6 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="185">
   <si>
@@ -653,7 +630,7 @@
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
   <si>
-    <t>Additional Potential (GW)</t>
+    <t>We assume the additional potential is double BAU deployment.</t>
   </si>
 </sst>
 </file>
@@ -1744,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1888,7 +1865,9 @@
       <c r="B34" s="6"/>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="7"/>
+      <c r="A36" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3"/>
@@ -3336,42 +3315,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0901BFDC-7419-499F-8451-F914B4698FB9}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2020</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>2050</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK114"/>
   <sheetViews>
@@ -10663,14 +10606,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -10913,14 +10856,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:AF2"/>
     </sheetView>
   </sheetViews>
@@ -11032,129 +10975,129 @@
       <c r="A2" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="8" cm="1">
-        <f t="array" ref="B2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!B1)*1000</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="8" cm="1">
-        <f t="array" ref="C2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!C1)*1000</f>
-        <v>1666.6666666665151</v>
-      </c>
-      <c r="D2" s="8" cm="1">
-        <f t="array" ref="D2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!D1)*1000</f>
-        <v>3333.3333333330302</v>
-      </c>
-      <c r="E2" s="8" cm="1">
-        <f t="array" ref="E2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!E1)*1000</f>
-        <v>5000</v>
-      </c>
-      <c r="F2" s="8" cm="1">
-        <f t="array" ref="F2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!F1)*1000</f>
-        <v>6666.6666666665151</v>
-      </c>
-      <c r="G2" s="8" cm="1">
-        <f t="array" ref="G2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!G1)*1000</f>
-        <v>8333.3333333330302</v>
-      </c>
-      <c r="H2" s="8" cm="1">
-        <f t="array" ref="H2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!H1)*1000</f>
-        <v>10000</v>
-      </c>
-      <c r="I2" s="8" cm="1">
-        <f t="array" ref="I2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!I1)*1000</f>
-        <v>11666.666666666515</v>
-      </c>
-      <c r="J2" s="8" cm="1">
-        <f t="array" ref="J2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!J1)*1000</f>
-        <v>13333.33333333303</v>
-      </c>
-      <c r="K2" s="8" cm="1">
-        <f t="array" ref="K2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!K1)*1000</f>
-        <v>15000</v>
-      </c>
-      <c r="L2" s="8" cm="1">
-        <f t="array" ref="L2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!L1)*1000</f>
-        <v>16666.666666666515</v>
-      </c>
-      <c r="M2" s="8" cm="1">
-        <f t="array" ref="M2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!M1)*1000</f>
-        <v>18333.33333333303</v>
-      </c>
-      <c r="N2" s="8" cm="1">
-        <f t="array" ref="N2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!N1)*1000</f>
-        <v>20000</v>
-      </c>
-      <c r="O2" s="8" cm="1">
-        <f t="array" ref="O2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!O1)*1000</f>
-        <v>21666.666666666515</v>
-      </c>
-      <c r="P2" s="8" cm="1">
-        <f t="array" ref="P2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!P1)*1000</f>
-        <v>23333.33333333303</v>
-      </c>
-      <c r="Q2" s="8" cm="1">
-        <f t="array" ref="Q2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!Q1)*1000</f>
-        <v>25000</v>
-      </c>
-      <c r="R2" s="8" cm="1">
-        <f t="array" ref="R2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!R1)*1000</f>
-        <v>26666.666666666515</v>
-      </c>
-      <c r="S2" s="8" cm="1">
-        <f t="array" ref="S2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!S1)*1000</f>
-        <v>28333.33333333303</v>
-      </c>
-      <c r="T2" s="8" cm="1">
-        <f t="array" ref="T2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!T1)*1000</f>
-        <v>30000</v>
-      </c>
-      <c r="U2" s="8" cm="1">
-        <f t="array" ref="U2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!U1)*1000</f>
-        <v>31666.666666666515</v>
-      </c>
-      <c r="V2" s="8" cm="1">
-        <f t="array" ref="V2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!V1)*1000</f>
-        <v>33333.33333333303</v>
-      </c>
-      <c r="W2" s="8" cm="1">
-        <f t="array" ref="W2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!W1)*1000</f>
-        <v>35000</v>
-      </c>
-      <c r="X2" s="8" cm="1">
-        <f t="array" ref="X2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!X1)*1000</f>
-        <v>36666.666666666511</v>
-      </c>
-      <c r="Y2" s="8" cm="1">
-        <f t="array" ref="Y2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!Y1)*1000</f>
-        <v>38333.33333333303</v>
-      </c>
-      <c r="Z2" s="8" cm="1">
-        <f t="array" ref="Z2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!Z1)*1000</f>
-        <v>40000</v>
-      </c>
-      <c r="AA2" s="8" cm="1">
-        <f t="array" ref="AA2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AA1)*1000</f>
-        <v>41666.666666666511</v>
-      </c>
-      <c r="AB2" s="8" cm="1">
-        <f t="array" ref="AB2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AB1)*1000</f>
-        <v>43333.33333333303</v>
-      </c>
-      <c r="AC2" s="8" cm="1">
-        <f t="array" ref="AC2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AC1)*1000</f>
-        <v>45000</v>
-      </c>
-      <c r="AD2" s="8" cm="1">
-        <f t="array" ref="AD2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AD1)*1000</f>
-        <v>46666.666666666511</v>
-      </c>
-      <c r="AE2" s="8" cm="1">
-        <f t="array" ref="AE2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AE1)*1000</f>
-        <v>48333.33333333303</v>
-      </c>
-      <c r="AF2" s="8" cm="1">
-        <f t="array" ref="AF2">TREND(Sheet1!$B$3:$B$4,Sheet1!$A$3:$A$4,PAGBSC!AF1)*1000</f>
-        <v>50000</v>
+      <c r="B2" s="8">
+        <f>BGBSC!B2</f>
+        <v>2560.3333333333335</v>
+      </c>
+      <c r="C2" s="8">
+        <f>BGBSC!C2</f>
+        <v>2714.3383458646617</v>
+      </c>
+      <c r="D2" s="8">
+        <f>BGBSC!D2</f>
+        <v>2877.6068177963707</v>
+      </c>
+      <c r="E2" s="8">
+        <f>BGBSC!E2</f>
+        <v>3050.6959496938966</v>
+      </c>
+      <c r="F2" s="8">
+        <f>BGBSC!F2</f>
+        <v>3212.9670108478272</v>
+      </c>
+      <c r="G2" s="8">
+        <f>BGBSC!G2</f>
+        <v>3375.2380720017582</v>
+      </c>
+      <c r="H2" s="8">
+        <f>BGBSC!H2</f>
+        <v>3548.3272038992845</v>
+      </c>
+      <c r="I2" s="8">
+        <f>BGBSC!I2</f>
+        <v>4716.6788442075858</v>
+      </c>
+      <c r="J2" s="8">
+        <f>BGBSC!J2</f>
+        <v>6123.028040874985</v>
+      </c>
+      <c r="K2" s="8">
+        <f>BGBSC!K2</f>
+        <v>7778.1928646450779</v>
+      </c>
+      <c r="L2" s="8">
+        <f>BGBSC!L2</f>
+        <v>9649.7191032870778</v>
+      </c>
+      <c r="M2" s="8">
+        <f>BGBSC!M2</f>
+        <v>11683.516403083009</v>
+      </c>
+      <c r="N2" s="8">
+        <f>BGBSC!N2</f>
+        <v>13803.858268827704</v>
+      </c>
+      <c r="O2" s="8">
+        <f>BGBSC!O2</f>
+        <v>15913.382063828803</v>
+      </c>
+      <c r="P2" s="8">
+        <f>BGBSC!P2</f>
+        <v>17936.361292881142</v>
+      </c>
+      <c r="Q2" s="8">
+        <f>BGBSC!Q2</f>
+        <v>19793.926915662018</v>
+      </c>
+      <c r="R2" s="8">
+        <f>BGBSC!R2</f>
+        <v>21432.748419120435</v>
+      </c>
+      <c r="S2" s="8">
+        <f>BGBSC!S2</f>
+        <v>22824.362926100708</v>
+      </c>
+      <c r="T2" s="8">
+        <f>BGBSC!T2</f>
+        <v>23964.006435527936</v>
+      </c>
+      <c r="U2" s="8">
+        <f>BGBSC!U2</f>
+        <v>24865.944610694143</v>
+      </c>
+      <c r="V2" s="8">
+        <f>BGBSC!V2</f>
+        <v>25557.154392976972</v>
+      </c>
+      <c r="W2" s="8">
+        <f>BGBSC!W2</f>
+        <v>26071.033632088998</v>
+      </c>
+      <c r="X2" s="8">
+        <f>BGBSC!X2</f>
+        <v>26442.238985480832</v>
+      </c>
+      <c r="Y2" s="8">
+        <f>BGBSC!Y2</f>
+        <v>26703.109292459074</v>
+      </c>
+      <c r="Z2" s="8">
+        <f>BGBSC!Z2</f>
+        <v>26881.639665600382</v>
+      </c>
+      <c r="AA2" s="8">
+        <f>BGBSC!AA2</f>
+        <v>27000.699193812103</v>
+      </c>
+      <c r="AB2" s="8">
+        <f>BGBSC!AB2</f>
+        <v>27078.100174737534</v>
+      </c>
+      <c r="AC2" s="8">
+        <f>BGBSC!AC2</f>
+        <v>27127.159025832974</v>
+      </c>
+      <c r="AD2" s="8">
+        <f>BGBSC!AD2</f>
+        <v>27157.473073762176</v>
+      </c>
+      <c r="AE2" s="8">
+        <f>BGBSC!AE2</f>
+        <v>27175.729575421621</v>
+      </c>
+      <c r="AF2" s="8">
+        <f>BGBSC!AF2</f>
+        <v>27186.441512750134</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -11170,7 +11113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>

</xml_diff>